<commit_message>
Updated the files with mapping
</commit_message>
<xml_diff>
--- a/jcp-v2/04-rsconnectProfiles/SKU_Div1-20Feb_Small.xlsx
+++ b/jcp-v2/04-rsconnectProfiles/SKU_Div1-20Feb_Small.xlsx
@@ -113,68 +113,74 @@
     <t>COLOR:Sleet||SIZE:Small</t>
   </si>
   <si>
-    <t>Sku Id</t>
-  </si>
-  <si>
     <t>Creation Date</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
     <t>Display Name</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Sku Feed Id</t>
-  </si>
-  <si>
-    <t>Sku Nb</t>
-  </si>
-  <si>
     <t>Swatch Im Id</t>
   </si>
   <si>
-    <t>Stus Cd</t>
-  </si>
-  <si>
-    <t>Rtl Sku Nb</t>
-  </si>
-  <si>
-    <t>Hide Dspl In</t>
-  </si>
-  <si>
-    <t>Sku Typ Cd</t>
-  </si>
-  <si>
-    <t>Sku Qy</t>
-  </si>
-  <si>
-    <t>Barcode Cd</t>
-  </si>
-  <si>
-    <t>Sku Attributes</t>
-  </si>
-  <si>
-    <t>Product Id</t>
+    <t>Store OOS Date</t>
+  </si>
+  <si>
+    <t>eComm OOS Date</t>
+  </si>
+  <si>
+    <t>Source Feed</t>
+  </si>
+  <si>
+    <t>Sku Number</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Model Number</t>
+  </si>
+  <si>
+    <t>Hide Display</t>
+  </si>
+  <si>
+    <t>Special Item Code</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>SKU Grouping</t>
+  </si>
+  <si>
+    <t>Product Title</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,13 +203,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -487,7 +527,8 @@
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="135.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="135.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.33203125" bestFit="1" customWidth="1"/>
@@ -503,22 +544,22 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
       </c>
       <c r="G1" t="s">
         <v>35</v>
@@ -527,31 +568,31 @@
         <v>36</v>
       </c>
       <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>44</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -951,6 +992,13 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="Q1">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q1">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>